<commit_message>
Added account type and updated sql
</commit_message>
<xml_diff>
--- a/BeHisebe_DB.xlsx
+++ b/BeHisebe_DB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <t xml:space="preserve">BeHIsebe Database Design</t>
   </si>
@@ -37,6 +37,12 @@
     <t xml:space="preserve">primary key (int)</t>
   </si>
   <si>
+    <t xml:space="preserve">AccountType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foreign_key (int)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Master</t>
   </si>
   <si>
@@ -55,6 +61,18 @@
     <t xml:space="preserve">User might add some note. Optional</t>
   </si>
   <si>
+    <t xml:space="preserve">BankAccountType Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TINYINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Credit Table</t>
   </si>
   <si>
@@ -65,9 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">bank_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foreign_key (int)</t>
   </si>
   <si>
     <t xml:space="preserve">amount</t>
@@ -191,7 +206,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -241,6 +256,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -303,7 +323,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -352,11 +372,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,21 +481,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="56.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="56.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="36.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="2.51"/>
   </cols>
@@ -528,439 +560,439 @@
       <c r="D6" s="10"/>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="40.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="11.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
       <c r="B7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>7</v>
-      </c>
+      <c r="D7" s="10"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="40.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
       <c r="B8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10"/>
       <c r="E8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="10" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D9" s="10"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="12"/>
+      <c r="B10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
-      <c r="B11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
-      <c r="B12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="B12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8"/>
       <c r="D12" s="14" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="12.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="12.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>17</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" customFormat="false" ht="12.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
-      <c r="B15" s="12"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="12"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>19</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="10" t="s">
-        <v>20</v>
+      <c r="C17" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>19</v>
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="10" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="10"/>
+        <v>6</v>
+      </c>
+      <c r="D18" s="18"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="D19" s="18"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
-      <c r="B20" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>24</v>
-      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="12"/>
+      <c r="B21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="7" t="s">
-        <v>2</v>
       </c>
       <c r="E22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="10" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="D23" s="10"/>
       <c r="E23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>28</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D24" s="10"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="10"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
-      <c r="B26" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>32</v>
-      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
-      <c r="B27" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="10"/>
+      <c r="B27" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="E27" s="5"/>
     </row>
-    <row r="28" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="10" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="10"/>
+        <v>33</v>
+      </c>
       <c r="E29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="12"/>
+      <c r="B30" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="10"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="7" t="s">
-        <v>2</v>
       </c>
       <c r="E31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="10" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="D32" s="10"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
       <c r="B34" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
-      <c r="B35" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>41</v>
-      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="13"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
-      <c r="B36" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="10" t="s">
+      <c r="B36" s="7" t="s">
         <v>42</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="E36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
       <c r="B37" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="12"/>
+      <c r="B38" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="10"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="C39" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="10"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
       <c r="B40" s="10" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
       <c r="B41" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="E41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
       <c r="B42" s="10" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
-      <c r="B43" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="10"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="13"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="12"/>
+      <c r="B44" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
-      <c r="B45" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B45" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="10"/>
       <c r="E45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5"/>
       <c r="B46" s="10" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="D46" s="10"/>
       <c r="E46" s="5"/>
@@ -968,10 +1000,10 @@
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5"/>
       <c r="B47" s="10" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="5"/>
@@ -979,73 +1011,124 @@
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5"/>
       <c r="B48" s="10" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D48" s="10"/>
       <c r="E48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5"/>
-      <c r="B49" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" s="10"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="13"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="16"/>
+      <c r="B50" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="E50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5"/>
-      <c r="B51" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="13"/>
-      <c r="D51" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B51" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="10"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5"/>
       <c r="B52" s="10" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>51</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D52" s="10"/>
       <c r="E52" s="5"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5"/>
       <c r="B53" s="10" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="5"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="12"/>
+      <c r="B54" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" s="10"/>
       <c r="E54" s="5"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5"/>
+      <c r="B56" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5"/>
+      <c r="B57" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E57" s="5"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="5"/>
+      <c r="B58" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="10"/>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>